<commit_message>
Base de Datos de Alumnos y Docentes actualizada:
- Se mejoró la base de datos presente, para una mejor gestión y personalización del programa; se corrigieron los errores de acentuación, así mismo, solo se mantuvieron en mayúsculas las iniciales de cada nombre a utilizar.
</commit_message>
<xml_diff>
--- a/Docentes Episs.xlsx
+++ b/Docentes Episs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edson\Documents\GitHub\google-app-script-Unsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1FA0BB-A17C-45F7-A373-B4659D55FD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1685D3-289A-444F-A525-0EBECF97B254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="115">
   <si>
     <t>Nombres</t>
   </si>
@@ -47,331 +47,337 @@
     <t>Estudiantes</t>
   </si>
   <si>
-    <t>BEDREGAL ALPACA, NORKA NORALI</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>TALLERES DE PSICOLOGIA</t>
-  </si>
-  <si>
-    <t>CORRALES DELGADO, CARLO JOSE LUIS</t>
-  </si>
-  <si>
-    <t>Mg.</t>
-  </si>
-  <si>
-    <t>CALCULO EN VARIAS VARIABLES</t>
-  </si>
-  <si>
-    <t>ESCOBEDO QUISPE, RICHART SMITH</t>
-  </si>
-  <si>
-    <t>TALLER DE LIDERAZGO Y COLABORACION</t>
-  </si>
-  <si>
-    <t>GUEVARA PUENTE DE LA VEGA, KARIM</t>
-  </si>
-  <si>
-    <t>INNOVACION Y CREATIVIDAD</t>
-  </si>
-  <si>
-    <t>PEREZ VERA, YASIEL</t>
-  </si>
-  <si>
-    <t>PROGRAMACION WEB 2</t>
-  </si>
-  <si>
-    <t>VIDAL DUARTE, ELIZABETH ENRIQUETA</t>
-  </si>
-  <si>
-    <t>REDACCION DE ARTICULOS E INFORMES DE INVESTIGACION</t>
-  </si>
-  <si>
     <t>ESTRUCTURA DE DATOS Y ALGORITMOS</t>
   </si>
   <si>
-    <t>CIUDADANIA E INTERCULTURALIDAD</t>
-  </si>
-  <si>
-    <t>ALARICO PACHECO, CAMILA FERNANDA</t>
-  </si>
-  <si>
-    <t>ALIAGA CHAIÑA, SANDRA GABRIELA</t>
-  </si>
-  <si>
-    <t>ALVAREZ LLAVE, FABIAN ANDRE</t>
-  </si>
-  <si>
-    <t>APAZA ANAHUA, ROYDAN ARTEMIO</t>
-  </si>
-  <si>
-    <t>ARAGON CARPIO, FREDY JOSE</t>
-  </si>
-  <si>
-    <t>AUCCACUSI CONDE, BRAYAN CARLOS</t>
-  </si>
-  <si>
-    <t>AYQUE PURACA, TANIA LUZ</t>
-  </si>
-  <si>
-    <t>BACA CALSIN, LEONARDO JUAN JOSE</t>
-  </si>
-  <si>
-    <t>BEDREGAL COAGUILA, KARLA MILUSKA</t>
-  </si>
-  <si>
-    <t>BRAVO ARREDONDO, CRISTHIAN MATIAS</t>
-  </si>
-  <si>
-    <t>CAMARGO HILACHOQUE, ROMINA GIULIANA</t>
-  </si>
-  <si>
-    <t>CARACELA CHALLCO, ANTHONY JEFFRY</t>
-  </si>
-  <si>
-    <t>CARLOS CCAMAQQUE, WILSON FREDDY</t>
-  </si>
-  <si>
-    <t>CARRILLO VILLALTA, GUSTAVO ALONSO</t>
-  </si>
-  <si>
-    <t>CASTELLANOS AMPUERO, BASILY ANDREE</t>
-  </si>
-  <si>
-    <t>CHAVEZ CUNO, DEIVICK PAUL EDDI</t>
-  </si>
-  <si>
-    <t>CHIPANA JERONIMO, GERMAN ARTURO</t>
-  </si>
-  <si>
-    <t>CHIPANA MAMANI, ANDHY BRAYAN</t>
-  </si>
-  <si>
-    <t>CHIRINOS ROJAS, KENNEDY</t>
-  </si>
-  <si>
-    <t>CHOQUE SANCHEZ, ALEJANDRA CAMILA</t>
-  </si>
-  <si>
-    <t>CHOQUEHUANCA BEDOYA, BRAYAN DENILSON</t>
-  </si>
-  <si>
-    <t>CHOQUEHUANCA BERNA, WILLIAM HERDERSON</t>
-  </si>
-  <si>
-    <t>COAQUIRA SUYO, GABRIELA DAYANA</t>
-  </si>
-  <si>
-    <t>CONDORI CAIRA, ANTONY BELTRAN</t>
-  </si>
-  <si>
-    <t>CONDORI CATUNTA, JOSELIN SHARON</t>
-  </si>
-  <si>
-    <t>CONDORI IDME, RAUL WILFREDO</t>
-  </si>
-  <si>
-    <t>CORNEJO HURTADO, DARIO RAFAEL</t>
-  </si>
-  <si>
-    <t>CUYO CCAPA, JHON DEYVIS</t>
-  </si>
-  <si>
-    <t>DAVILA FLORES, MATHIAS DARIO</t>
-  </si>
-  <si>
-    <t>ESTRADA ARCE, SERGIO EMILIO</t>
-  </si>
-  <si>
-    <t>ESTEFANERO PALMA, RODRIGO</t>
-  </si>
-  <si>
-    <t>FIGUEROA LARUTA, SUEMY ALEXANDRA</t>
-  </si>
-  <si>
-    <t>FLORES NUÑEZ, RODRIGO FRANCISCO</t>
-  </si>
-  <si>
-    <t>GUERRA PILCO, WILBER JESUS</t>
-  </si>
-  <si>
-    <t>GUILLEN VALCARCEL, DANIEL JOSUE</t>
-  </si>
-  <si>
-    <t>HATCHES CURO, JOSE LEON ENRIQUE</t>
-  </si>
-  <si>
-    <t>HILACONDO BEGAZO, EMANUEL DAVID</t>
-  </si>
-  <si>
-    <t>HUAYNACHO MANGO, JERRY ANDERSON</t>
-  </si>
-  <si>
-    <t>IGREDA ALVARADO, JAIME DANIEL</t>
-  </si>
-  <si>
-    <t>JIMENEZ PAREDES, FABRICIO GABRIEL</t>
-  </si>
-  <si>
-    <t>LAYME SALAS, RODRIGO FABRICIO</t>
-  </si>
-  <si>
-    <t>LEON RAMOS, MIJAEL PAUL</t>
-  </si>
-  <si>
-    <t>LLAIQUE CHULLUNQUIA, JACK FRANCO</t>
-  </si>
-  <si>
-    <t>LLAVE AGUILAR, JAFET MARTIN</t>
-  </si>
-  <si>
-    <t>LLAVILLA MACHACA, FRAYD YANDEL</t>
-  </si>
-  <si>
-    <t>LUQUE GUEVARA, FERNANDO GERSON</t>
-  </si>
-  <si>
-    <t>MAMANI QUISPE, RENZO GEOMAR</t>
-  </si>
-  <si>
-    <t>MAYTA QUISPE, PAOLA ADAMARI</t>
-  </si>
-  <si>
-    <t>MEJIA RONDAN, GIOVANNI PATRICK</t>
-  </si>
-  <si>
-    <t>MELENDEZ RAVELLO, EDUARDO FREDY</t>
-  </si>
-  <si>
-    <t>MENGOA VALERIANO, BRIGITTE NOELIA</t>
-  </si>
-  <si>
-    <t>MOROCCO SAICO, JOSE MANUEL</t>
-  </si>
-  <si>
-    <t>OCHOA RIEGA, SAUL BASTIAN ALESSANDRO</t>
-  </si>
-  <si>
-    <t>ORE SOTO, ANDRES RAUL</t>
-  </si>
-  <si>
-    <t>PACHECO MEDINA, GEISEL REYMAR</t>
-  </si>
-  <si>
-    <t>PALMA APAZA, SANTIAGO ENRIQUE</t>
-  </si>
-  <si>
-    <t>PAREDES MIRANDA, MAURICIO ANTONIO</t>
-  </si>
-  <si>
-    <t>PONCE LLERENA, RENATO XAVIER</t>
-  </si>
-  <si>
-    <t>QUENTA AHUMADA, PAULO ESTEFANO</t>
-  </si>
-  <si>
-    <t>QUISPE BEDREGAL, JOAQUIN ALEJANDRO</t>
-  </si>
-  <si>
-    <t>QUISPE MAMANI, JOSE GABRIEL</t>
-  </si>
-  <si>
-    <t>QUISPE PAUCCAR, JOSUE CLAUDIO</t>
-  </si>
-  <si>
-    <t>QUISPE PUMA, USIEL SURIEL</t>
-  </si>
-  <si>
-    <t>QUISPE RUPAYLLA, FABRIZIO ALONSO</t>
-  </si>
-  <si>
-    <t>QUISPESAYHUA HANCCO, JOSEPH BRAYAN</t>
-  </si>
-  <si>
-    <t>RIVAS REVILLA, DIEGO EDUARDO</t>
-  </si>
-  <si>
-    <t>RIVEROS VILCA, ALBERTH EDWAR</t>
-  </si>
-  <si>
-    <t>ROJAS CONDORI, FABIANA PAOLA</t>
-  </si>
-  <si>
-    <t>SAAVEDRA INGA, GONZALO DE ALESANDRO</t>
-  </si>
-  <si>
-    <t>SANTA CRUZ VILLA, DIEGO SEBASTIAN</t>
-  </si>
-  <si>
-    <t>SCHREIBER LANDEO, DIEGO HANS</t>
-  </si>
-  <si>
-    <t>SILVA PINO, JESUS FRANCISCO</t>
-  </si>
-  <si>
-    <t>SIVINCHA MACHACA, SAUL ANDRE</t>
-  </si>
-  <si>
-    <t>SOLSOL CHOQUE, FERNANDO RAFAEL</t>
-  </si>
-  <si>
-    <t>SONCCO HANCCO, PEDRO MIGUEL</t>
-  </si>
-  <si>
-    <t>SORIA SONCCO, RODOLFO PAUL</t>
-  </si>
-  <si>
-    <t>SOTA ZEBALLOS, ALEXIS HUMBERTO</t>
-  </si>
-  <si>
-    <t>SUBIA HUAICANE, EDSON FABRICIO</t>
-  </si>
-  <si>
-    <t>SULLCA MAMANI, MAURO SNAYDER</t>
-  </si>
-  <si>
-    <t>TICLLAHUANACO HUACHO, PERCY ORLANDO</t>
-  </si>
-  <si>
-    <t>TICONA SAURE, JOSE MARIA</t>
-  </si>
-  <si>
-    <t>TIJERO DAVILA, JEIC LUCCIANO VALENTINO</t>
-  </si>
-  <si>
-    <t>ULLOA SALAS, SEBASTIAN DONATO</t>
-  </si>
-  <si>
-    <t>VELAZQUE QUISPE, FLOR DE LIZ</t>
-  </si>
-  <si>
-    <t>VILCA FLORES, JOHAN HUGO</t>
-  </si>
-  <si>
-    <t>VILCA MAMANI, JOSE ARMANDO</t>
-  </si>
-  <si>
-    <t>VILCAPE ROSAS, EDITH LUCERO</t>
-  </si>
-  <si>
-    <t>YANA HUANCA, CHRISTIAN ALEXANDER</t>
-  </si>
-  <si>
-    <t>YAULI MERMA, DIEGO RAUL</t>
-  </si>
-  <si>
-    <t>ZAMBRANO CRUZ, YSABEL ALEJANDRA</t>
-  </si>
-  <si>
-    <t>SULLA TORRES, JOSÉ ALFREDO</t>
-  </si>
-  <si>
-    <t>TARQUI AYALA, JORGE WASHINGTON</t>
-  </si>
-  <si>
-    <t>PEÑALVA SUCA, LORENZO JESÚS</t>
+    <t>CÁLCULO EN VARIAS VARIABLES</t>
+  </si>
+  <si>
+    <t>INNOVACIÓN Y CREATIVIDAD</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN WEB 2</t>
+  </si>
+  <si>
+    <t>REDACCIÓN DE ARTÍCULOS E INFORMES DE INVESTIGACIÓN</t>
+  </si>
+  <si>
+    <t>CIUDADANÍA E INTERCULTURALIDAD</t>
+  </si>
+  <si>
+    <t>TALLER DE LIDERAZGO Y COLABORACIÓN</t>
+  </si>
+  <si>
+    <t>TALLERES DE PSICOLOGÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg. </t>
+  </si>
+  <si>
+    <t>Alarico Pacheco, Camila Fernanda</t>
+  </si>
+  <si>
+    <t>Aliaga Chaiña, Sandra Gabriela</t>
+  </si>
+  <si>
+    <t>Álvarez Llave, Fabián André</t>
+  </si>
+  <si>
+    <t>Apaza Anahua, Roydan Artemio</t>
+  </si>
+  <si>
+    <t>Aragón Carpio, Fredy José</t>
+  </si>
+  <si>
+    <t>Auccacusi Conde, Brayan Carlos</t>
+  </si>
+  <si>
+    <t>Ayque Puraca, Tania Luz</t>
+  </si>
+  <si>
+    <t>Baca Calsín, Leonardo Juan José</t>
+  </si>
+  <si>
+    <t>Bedregal Coaguila, Karla Miluska</t>
+  </si>
+  <si>
+    <t>Bravo Arredondo, Cristhian Matías</t>
+  </si>
+  <si>
+    <t>Camargo Hilachoque, Romina Giuliana</t>
+  </si>
+  <si>
+    <t>Caracela Challco, Anthony Jeffry</t>
+  </si>
+  <si>
+    <t>Carlos Ccamaqque, Wilson Freddy</t>
+  </si>
+  <si>
+    <t>Carrillo Villalta, Gustavo Alonso</t>
+  </si>
+  <si>
+    <t>Castellanos Ampuero, Basily Andrée</t>
+  </si>
+  <si>
+    <t>Chávez Cuño, Deivick Paul Eddi</t>
+  </si>
+  <si>
+    <t>Chipana Jerónimo, Germán Arturo</t>
+  </si>
+  <si>
+    <t>Chipana Mamani, Andhy Brayan</t>
+  </si>
+  <si>
+    <t>Chirinos Rojas, Kennedy</t>
+  </si>
+  <si>
+    <t>Choque Sánchez, Alejandra Camila</t>
+  </si>
+  <si>
+    <t>Choquehuanca Bedoya, Brayan Denilson</t>
+  </si>
+  <si>
+    <t>Choquehuanca Berna, William Herderson</t>
+  </si>
+  <si>
+    <t>Coaquira Suyo, Gabriela Dayana</t>
+  </si>
+  <si>
+    <t>Condori Caira, Antony Beltrán</t>
+  </si>
+  <si>
+    <t>Condori Catunta, Joselín Sharon</t>
+  </si>
+  <si>
+    <t>Condori Idme, Raúl Wilfredo</t>
+  </si>
+  <si>
+    <t>Cornejo Hurtado, Darío Rafael</t>
+  </si>
+  <si>
+    <t>Corrales Delgado, Carlo José Luis</t>
+  </si>
+  <si>
+    <t>Cuyo Ccapa, Jhon Deyvis</t>
+  </si>
+  <si>
+    <t>Dávila Flores, Mathias Darío</t>
+  </si>
+  <si>
+    <t>Estrada Arce, Sergio Emilio</t>
+  </si>
+  <si>
+    <t>Estefanero Palma, Rodrigo</t>
+  </si>
+  <si>
+    <t>Figueroa Laruta, Suemy Alexandra</t>
+  </si>
+  <si>
+    <t>Flores Núñez, Rodrigo Francisco</t>
+  </si>
+  <si>
+    <t>Guevara Puente de la Vega, Karim</t>
+  </si>
+  <si>
+    <t>Guerra Pilco, Wilber Jesús</t>
+  </si>
+  <si>
+    <t>Guillén Valcárcel, Daniel Josué</t>
+  </si>
+  <si>
+    <t>Hatches Curo, José León Enrique</t>
+  </si>
+  <si>
+    <t>Hilacondo Begazo, Emanuel David</t>
+  </si>
+  <si>
+    <t>Huaynacho Mango, Jerry Anderson</t>
+  </si>
+  <si>
+    <t>Igreda Alvarado, Jaime Daniel</t>
+  </si>
+  <si>
+    <t>Jiménez Paredes, Fabricio Gabriel</t>
+  </si>
+  <si>
+    <t>Layme Salas, Rodrigo Fabricio</t>
+  </si>
+  <si>
+    <t>León Ramos, Mijael Paul</t>
+  </si>
+  <si>
+    <t>Llaique Chullunquia, Jack Franco</t>
+  </si>
+  <si>
+    <t>Llave Aguilar, Jafet Martín</t>
+  </si>
+  <si>
+    <t>Llavilla Machaca, Frayd Yandel</t>
+  </si>
+  <si>
+    <t>Luque Guevara, Fernando Gerson</t>
+  </si>
+  <si>
+    <t>Mamani Quispe, Renzo Geomar</t>
+  </si>
+  <si>
+    <t>Mayta Quispe, Paola Adamari</t>
+  </si>
+  <si>
+    <t>Mejía Rondán, Giovanni Patrick</t>
+  </si>
+  <si>
+    <t>Meléndez Ravello, Eduardo Fredy</t>
+  </si>
+  <si>
+    <t>Mengoa Valeriano, Brigitte Noelia</t>
+  </si>
+  <si>
+    <t>Morocco Saico, José Manuel</t>
+  </si>
+  <si>
+    <t>Ochoa Riega, Saúl Bastián Alessandro</t>
+  </si>
+  <si>
+    <t>Oré Soto, Andrés Raúl</t>
+  </si>
+  <si>
+    <t>Pacheco Medina, Geisel Reymar</t>
+  </si>
+  <si>
+    <t>Palma Apaza, Santiago Enrique</t>
+  </si>
+  <si>
+    <t>Paredes Miranda, Mauricio Antonio</t>
+  </si>
+  <si>
+    <t>Ponce Llerena, Renato Xavier</t>
+  </si>
+  <si>
+    <t>Quenta Ahumada, Paulo Estéfano</t>
+  </si>
+  <si>
+    <t>Quispe Bedregal, Joaquín Alejandro</t>
+  </si>
+  <si>
+    <t>Quispe Mamani, José Gabriel</t>
+  </si>
+  <si>
+    <t>Quispe Pauccar, Josué Claudio</t>
+  </si>
+  <si>
+    <t>Quispe Puma, Usiel Suriel</t>
+  </si>
+  <si>
+    <t>Quispe Rupaylla, Fabrizio Alonso</t>
+  </si>
+  <si>
+    <t>Quispesayhua Hancco, Joseph Brayan</t>
+  </si>
+  <si>
+    <t>Rivas Revilla, Diego Eduardo</t>
+  </si>
+  <si>
+    <t>Riveros Vilca, Alberth Edwar</t>
+  </si>
+  <si>
+    <t>Rojas Condori, Fabiana Paola</t>
+  </si>
+  <si>
+    <t>Saavedra Inga, Gonzalo de Alesandro</t>
+  </si>
+  <si>
+    <t>Santa Cruz Villa, Diego Sebastián</t>
+  </si>
+  <si>
+    <t>Schreiber Landeo, Diego Hans</t>
+  </si>
+  <si>
+    <t>Silva Pino, Jesús Francisco</t>
+  </si>
+  <si>
+    <t>Sivincha Machaca, Saúl André</t>
+  </si>
+  <si>
+    <t>Solsol Choque, Fernando Rafael</t>
+  </si>
+  <si>
+    <t>Soncco Hancco, Pedro Miguel</t>
+  </si>
+  <si>
+    <t>Soria Soncco, Rodolfo Paul</t>
+  </si>
+  <si>
+    <t>Sota Zeballos, Alexis Humberto</t>
+  </si>
+  <si>
+    <t>Subia Huaicane, Edson Fabricio</t>
+  </si>
+  <si>
+    <t>Sullca Mamani, Mauro Snayder</t>
+  </si>
+  <si>
+    <t>Ticllahuanaco Huacho, Percy Orlando</t>
+  </si>
+  <si>
+    <t>Ticona Saure, José María</t>
+  </si>
+  <si>
+    <t>Tijero Dávila, Jeic Lucciano Valentino</t>
+  </si>
+  <si>
+    <t>Ulloa Salas, Sebastián Donato</t>
+  </si>
+  <si>
+    <t>Vilca Flores, Johan Hugo</t>
+  </si>
+  <si>
+    <t>Vilca Mamani, José Armando</t>
+  </si>
+  <si>
+    <t>Vilcape Rosas, Edith Lucero</t>
+  </si>
+  <si>
+    <t>Yana Huanca, Christian Alexander</t>
+  </si>
+  <si>
+    <t>Yauli Merma, Diego Raúl</t>
+  </si>
+  <si>
+    <t>Zambrano Cruz, Ysabel Alejandra</t>
+  </si>
+  <si>
+    <t>Velazque Quispe, Flor de Liz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedregal Alpaca, Norka Norali  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrales Delgado, Carlo José Luis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escobedo Quispe, Richart Smith  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guevara Puente de la Vega, Karim  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pérez Vera, Yasiel  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidal Duarte, Elizabeth Enriqueta  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarqui Ayala, Jorge Washington  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulla Torres, José Alfredo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peñalva Suca, Lorenzo Jesús  </t>
   </si>
 </sst>
 </file>
@@ -450,12 +456,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -682,7 +687,7 @@
   <dimension ref="A1:E171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,396 +713,396 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
+      <c r="A8" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>5</v>
+      <c r="A9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
+      <c r="A10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f>_xlfn.CONCAT(B4,A4)</f>
-        <v>Mg.ESCOBEDO QUISPE, RICHART SMITH</v>
+        <v xml:space="preserve">Mg. Escobedo Quispe, Richart Smith  </v>
       </c>
       <c r="B12" s="3"/>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f>_xlfn.CONCAT(B5,A5)</f>
-        <v>Dr.GUEVARA PUENTE DE LA VEGA, KARIM</v>
+        <v xml:space="preserve">Dr. Guevara Puente de la Vega, Karim  </v>
       </c>
       <c r="B13" s="3"/>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f>_xlfn.CONCAT(B6,A6)</f>
-        <v>Dr.PEREZ VERA, YASIEL</v>
+        <v xml:space="preserve">Dr. Pérez Vera, Yasiel  </v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f>_xlfn.CONCAT(B7,A7)</f>
-        <v>Dr.VIDAL DUARTE, ELIZABETH ENRIQUETA</v>
+        <v xml:space="preserve">Dr. Vidal Duarte, Elizabeth Enriqueta  </v>
       </c>
       <c r="B15" s="3"/>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f>_xlfn.CONCAT(B8,A8)</f>
-        <v>Mg.TARQUI AYALA, JORGE WASHINGTON</v>
+        <v xml:space="preserve">Mg. Tarqui Ayala, Jorge Washington  </v>
       </c>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f>_xlfn.CONCAT(B3,A3)</f>
-        <v>Mg.CORRALES DELGADO, CARLO JOSE LUIS</v>
+        <v xml:space="preserve">Mg. Corrales Delgado, Carlo José Luis  </v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f>_xlfn.SINGLE(_xlfn.CONCAT(B2,A2))</f>
-        <v>Dr.BEDREGAL ALPACA, NORKA NORALI</v>
+        <v xml:space="preserve">Dr. Bedregal Alpaca, Norka Norali  </v>
       </c>
       <c r="B18" s="3"/>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f>_xlfn.CONCAT(B10,A10)</f>
-        <v>Dr.PEÑALVA SUCA, LORENZO JESÚS</v>
+        <v xml:space="preserve">Dr. Peñalva Suca, Lorenzo Jesús  </v>
       </c>
       <c r="B19" s="3"/>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f>_xlfn.CONCAT(B9,A9)</f>
-        <v>Dr.SULLA TORRES, JOSÉ ALFREDO</v>
+        <v xml:space="preserve">Dr. Sulla Torres, José Alfredo  </v>
       </c>
       <c r="B20" s="3"/>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="D42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E46" s="4"/>
     </row>
@@ -1105,7 +1110,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E47" s="4"/>
     </row>
@@ -1113,7 +1118,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E48" s="4"/>
     </row>
@@ -1121,7 +1126,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E49" s="4"/>
     </row>
@@ -1129,7 +1134,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E50" s="4"/>
     </row>
@@ -1137,7 +1142,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="D51" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E51" s="4"/>
     </row>
@@ -1145,7 +1150,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E52" s="4"/>
     </row>
@@ -1153,7 +1158,7 @@
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="D53" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E53" s="4"/>
     </row>
@@ -1161,7 +1166,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="D54" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E54" s="4"/>
     </row>
@@ -1169,7 +1174,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="D55" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E55" s="4"/>
     </row>
@@ -1177,7 +1182,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="D56" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E56" s="4"/>
     </row>
@@ -1185,7 +1190,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E57" s="4"/>
     </row>
@@ -1193,7 +1198,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="D58" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E58" s="4"/>
     </row>
@@ -1201,7 +1206,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="D59" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -1209,7 +1214,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="D60" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E60" s="4"/>
     </row>
@@ -1217,7 +1222,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="D61" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E61" s="4"/>
     </row>
@@ -1225,7 +1230,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="D62" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E62" s="4"/>
     </row>
@@ -1233,7 +1238,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="D63" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E63" s="4"/>
     </row>
@@ -1241,7 +1246,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="D64" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E64" s="4"/>
     </row>
@@ -1249,7 +1254,7 @@
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E65" s="4"/>
     </row>
@@ -1257,7 +1262,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="D66" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E66" s="4"/>
     </row>
@@ -1265,7 +1270,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E67" s="4"/>
     </row>
@@ -1273,7 +1278,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E68" s="4"/>
     </row>
@@ -1281,7 +1286,7 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="D69" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E69" s="4"/>
     </row>
@@ -1289,386 +1294,383 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E70" s="4"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E72" s="4"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E74" s="4"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E78" s="4"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D80" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E81" s="4"/>
     </row>
     <row r="82" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E83" s="4"/>
     </row>
     <row r="84" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E86" s="4"/>
     </row>
     <row r="87" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E88" s="4"/>
     </row>
     <row r="89" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E89" s="4"/>
     </row>
     <row r="90" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
-        <v>106</v>
-      </c>
-      <c r="E90" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="E90" s="4"/>
     </row>
     <row r="91" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
-        <v>107</v>
-      </c>
-      <c r="E91" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="E91" s="4"/>
     </row>
     <row r="92" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D92" t="s">
-        <v>108</v>
-      </c>
-      <c r="E92" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="E92" s="4"/>
     </row>
     <row r="93" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
-        <v>109</v>
-      </c>
-      <c r="E93" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E94" s="5"/>
+      <c r="E94" s="4"/>
     </row>
     <row r="95" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E95" s="5"/>
+      <c r="E95" s="4"/>
     </row>
     <row r="96" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E96" s="5"/>
+      <c r="E96" s="4"/>
     </row>
     <row r="97" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E97" s="5"/>
+      <c r="E97" s="4"/>
     </row>
     <row r="98" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E98" s="5"/>
+      <c r="E98" s="4"/>
     </row>
     <row r="99" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E99" s="5"/>
+      <c r="E99" s="4"/>
     </row>
     <row r="100" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E100" s="5"/>
+      <c r="E100" s="4"/>
     </row>
     <row r="101" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E101" s="5"/>
+      <c r="E101" s="4"/>
     </row>
     <row r="102" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E102" s="5"/>
+      <c r="E102" s="4"/>
     </row>
     <row r="103" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E103" s="5"/>
+      <c r="E103" s="4"/>
     </row>
     <row r="104" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E104" s="5"/>
+      <c r="E104" s="4"/>
     </row>
     <row r="105" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E105" s="5"/>
+      <c r="E105" s="4"/>
     </row>
     <row r="106" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E106" s="5"/>
+      <c r="E106" s="4"/>
     </row>
     <row r="107" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E107" s="5"/>
+      <c r="E107" s="4"/>
     </row>
     <row r="108" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E108" s="5"/>
+      <c r="E108" s="4"/>
     </row>
     <row r="109" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E109" s="5"/>
+      <c r="E109" s="4"/>
     </row>
     <row r="110" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E110" s="5"/>
+      <c r="E110" s="4"/>
     </row>
     <row r="111" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E111" s="5"/>
+      <c r="E111" s="4"/>
     </row>
     <row r="112" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E112" s="5"/>
+      <c r="E112" s="4"/>
     </row>
     <row r="113" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E113" s="5"/>
+      <c r="E113" s="4"/>
     </row>
     <row r="114" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E114" s="5"/>
+      <c r="E114" s="4"/>
     </row>
     <row r="115" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E115" s="5"/>
+      <c r="E115" s="4"/>
     </row>
     <row r="116" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E116" s="5"/>
+      <c r="E116" s="4"/>
     </row>
     <row r="117" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="5"/>
+      <c r="E117" s="4"/>
     </row>
     <row r="118" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E118" s="5"/>
+      <c r="E118" s="4"/>
     </row>
     <row r="119" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E119" s="5"/>
+      <c r="E119" s="4"/>
     </row>
     <row r="120" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E120" s="5"/>
+      <c r="E120" s="4"/>
     </row>
     <row r="121" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E121" s="5"/>
+      <c r="E121" s="4"/>
     </row>
     <row r="122" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E122" s="5"/>
+      <c r="E122" s="4"/>
     </row>
     <row r="123" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E123" s="5"/>
+      <c r="E123" s="4"/>
     </row>
     <row r="124" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E124" s="5"/>
+      <c r="E124" s="4"/>
     </row>
     <row r="125" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E125" s="5"/>
+      <c r="E125" s="4"/>
     </row>
     <row r="126" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E126" s="5"/>
+      <c r="E126" s="4"/>
     </row>
     <row r="127" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E127" s="5"/>
+      <c r="E127" s="4"/>
     </row>
     <row r="128" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E128" s="5"/>
+      <c r="E128" s="4"/>
     </row>
     <row r="129" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E129" s="5"/>
+      <c r="E129" s="4"/>
     </row>
     <row r="130" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E130" s="5"/>
+      <c r="E130" s="4"/>
     </row>
     <row r="131" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E131" s="5"/>
+      <c r="E131" s="4"/>
     </row>
     <row r="132" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E132" s="5"/>
+      <c r="E132" s="4"/>
     </row>
     <row r="133" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E133" s="5"/>
+      <c r="E133" s="4"/>
     </row>
     <row r="134" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E134" s="5"/>
+      <c r="E134" s="4"/>
     </row>
     <row r="135" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E135" s="5"/>
+      <c r="E135" s="4"/>
     </row>
     <row r="136" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E136" s="5"/>
+      <c r="E136" s="4"/>
     </row>
     <row r="137" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E137" s="5"/>
+      <c r="E137" s="4"/>
     </row>
     <row r="138" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E138" s="5"/>
+      <c r="E138" s="4"/>
     </row>
     <row r="139" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E139" s="5"/>
+      <c r="E139" s="4"/>
     </row>
     <row r="140" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E140" s="5"/>
+      <c r="E140" s="4"/>
     </row>
     <row r="141" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E141" s="5"/>
+      <c r="E141" s="4"/>
     </row>
     <row r="142" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E142" s="5"/>
+      <c r="E142" s="4"/>
     </row>
     <row r="143" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E143" s="5"/>
+      <c r="E143" s="4"/>
     </row>
     <row r="144" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E144" s="5"/>
+      <c r="E144" s="4"/>
     </row>
     <row r="145" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E145" s="5"/>
+      <c r="E145" s="4"/>
     </row>
     <row r="146" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E146" s="5"/>
+      <c r="E146" s="4"/>
     </row>
     <row r="147" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E147" s="5"/>
+      <c r="E147" s="4"/>
     </row>
     <row r="148" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E148" s="5"/>
+      <c r="E148" s="4"/>
     </row>
     <row r="149" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E149" s="5"/>
+      <c r="E149" s="4"/>
     </row>
     <row r="150" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E150" s="5"/>
+      <c r="E150" s="4"/>
     </row>
     <row r="151" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E151" s="5"/>
+      <c r="E151" s="4"/>
     </row>
     <row r="152" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E152" s="5"/>
+      <c r="E152" s="4"/>
     </row>
     <row r="153" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E153" s="5"/>
+      <c r="E153" s="4"/>
     </row>
     <row r="154" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E154" s="5"/>
+      <c r="E154" s="4"/>
     </row>
     <row r="155" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E155" s="5"/>
+      <c r="E155" s="4"/>
     </row>
     <row r="156" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E156" s="5"/>
+      <c r="E156" s="4"/>
     </row>
     <row r="157" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E157" s="5"/>
+      <c r="E157" s="4"/>
     </row>
     <row r="158" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E158" s="5"/>
+      <c r="E158" s="4"/>
     </row>
     <row r="159" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E159" s="5"/>
+      <c r="E159" s="4"/>
     </row>
     <row r="160" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E160" s="5"/>
+      <c r="E160" s="4"/>
     </row>
     <row r="161" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E161" s="5"/>
+      <c r="E161" s="4"/>
     </row>
     <row r="162" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E162" s="5"/>
+      <c r="E162" s="4"/>
     </row>
     <row r="163" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E163" s="5"/>
+      <c r="E163" s="4"/>
     </row>
     <row r="164" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E164" s="5"/>
+      <c r="E164" s="4"/>
     </row>
     <row r="165" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E165" s="5"/>
+      <c r="E165" s="4"/>
     </row>
     <row r="166" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E166" s="5"/>
+      <c r="E166" s="4"/>
     </row>
     <row r="167" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E167" s="5"/>
+      <c r="E167" s="4"/>
     </row>
     <row r="168" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E168" s="5"/>
+      <c r="E168" s="4"/>
     </row>
     <row r="169" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E169" s="5"/>
+      <c r="E169" s="4"/>
     </row>
     <row r="170" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E170" s="5"/>
+      <c r="E170" s="4"/>
     </row>
     <row r="171" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E171" s="5"/>
+      <c r="E171" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" display="https://aulavirtual.unsa.edu.pe/2025A/user/view.php?id=628&amp;course=543" xr:uid="{E5AB07ED-7991-4C99-8F72-786F2670B0CC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>